<commit_message>
sn: update pretas form
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/july 2021/sn_lf_pretas_1_sites_202107.xlsx
+++ b/LF/PreTAS/Senegal/july 2021/sn_lf_pretas_1_sites_202107.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Senegal\july 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7848511-ECC3-459D-9DED-F3531AFC9F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7CB918-EC0A-4FC5-9114-84F333C4B872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13" yWindow="13" windowWidth="25587" windowHeight="13787" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -353,12 +353,6 @@
     <t>region_list</t>
   </si>
   <si>
-    <t>(Juillet 2021) 1. Pre-TAS FL - Formulaire Site</t>
-  </si>
-  <si>
-    <t>sn_lf_pretas_1_sites_202107</t>
-  </si>
-  <si>
     <t>Bignona</t>
   </si>
   <si>
@@ -539,9 +533,6 @@
     <t>SS Kholpa</t>
   </si>
   <si>
-    <t>SS Koba</t>
-  </si>
-  <si>
     <t>SS Kokolé</t>
   </si>
   <si>
@@ -582,6 +573,15 @@
   </si>
   <si>
     <t>${c_consent} = 'Non'</t>
+  </si>
+  <si>
+    <t>Sindialon</t>
+  </si>
+  <si>
+    <t>sn_lf_pretas_1_sites_202107_v2</t>
+  </si>
+  <si>
+    <t>(Juillet 2021) 1. Pre-TAS FL - Formulaire Site V2</t>
   </si>
 </sst>
 </file>
@@ -1207,17 +1207,17 @@
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
@@ -1260,7 +1260,7 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1405,7 +1405,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="9" t="s">
@@ -1435,7 +1435,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L10" s="14"/>
       <c r="M10" s="9" t="s">
@@ -1469,7 +1469,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="9" t="s">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="F12" s="19"/>
       <c r="K12" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="M12" s="30"/>
     </row>
@@ -1583,9 +1583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B138" sqref="B138"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -1864,13 +1864,13 @@
         <v>73</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>105</v>
@@ -1883,13 +1883,13 @@
         <v>73</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>99</v>
@@ -1902,13 +1902,13 @@
         <v>73</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>98</v>
@@ -1921,13 +1921,13 @@
         <v>73</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>98</v>
@@ -1940,13 +1940,13 @@
         <v>73</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>98</v>
@@ -1959,13 +1959,13 @@
         <v>73</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>72</v>
@@ -1978,13 +1978,13 @@
         <v>73</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>100</v>
@@ -2012,13 +2012,13 @@
         <v>73</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>99</v>
@@ -2029,13 +2029,13 @@
         <v>73</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E26" s="33" t="s">
         <v>72</v>
@@ -2046,13 +2046,13 @@
         <v>73</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E27" s="33" t="s">
         <v>99</v>
@@ -2063,13 +2063,13 @@
         <v>73</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E28" s="33" t="s">
         <v>71</v>
@@ -2080,13 +2080,13 @@
         <v>73</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E29" s="33" t="s">
         <v>98</v>
@@ -2097,13 +2097,13 @@
         <v>73</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>105</v>
@@ -2114,13 +2114,13 @@
         <v>73</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E31" s="33" t="s">
         <v>103</v>
@@ -2131,13 +2131,13 @@
         <v>73</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>104</v>
@@ -2148,13 +2148,13 @@
         <v>73</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>104</v>
@@ -2165,13 +2165,13 @@
         <v>73</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E34" s="33" t="s">
         <v>102</v>
@@ -2182,13 +2182,13 @@
         <v>73</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E35" s="33" t="s">
         <v>101</v>
@@ -2199,13 +2199,13 @@
         <v>73</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E36" s="33" t="s">
         <v>98</v>
@@ -2216,13 +2216,13 @@
         <v>73</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E37" s="33" t="s">
         <v>105</v>
@@ -2234,13 +2234,13 @@
         <v>73</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>97</v>
@@ -2278,17 +2278,17 @@
         <v>84</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E41" s="33"/>
       <c r="F41" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2296,17 +2296,17 @@
         <v>84</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E42" s="33"/>
       <c r="F42" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2314,17 +2314,17 @@
         <v>84</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E43" s="33"/>
       <c r="F43" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2332,17 +2332,17 @@
         <v>84</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E44" s="33"/>
       <c r="F44" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2350,17 +2350,17 @@
         <v>84</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E45" s="33"/>
       <c r="F45" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2368,17 +2368,17 @@
         <v>84</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E46" s="33"/>
       <c r="F46" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2386,17 +2386,17 @@
         <v>84</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E47" s="33"/>
       <c r="F47" s="32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2404,17 +2404,17 @@
         <v>84</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E48" s="33"/>
       <c r="F48" s="32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2422,13 +2422,13 @@
         <v>84</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E49" s="33"/>
       <c r="F49" s="32" t="s">
@@ -2440,17 +2440,17 @@
         <v>84</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E50" s="33"/>
       <c r="F50" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2458,17 +2458,17 @@
         <v>84</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E51" s="33"/>
       <c r="F51" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2476,17 +2476,17 @@
         <v>84</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E52" s="33"/>
       <c r="F52" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2494,17 +2494,17 @@
         <v>84</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E53" s="33"/>
       <c r="F53" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2512,17 +2512,17 @@
         <v>84</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E54" s="33"/>
       <c r="F54" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2530,17 +2530,17 @@
         <v>84</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E55" s="33"/>
       <c r="F55" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2548,17 +2548,17 @@
         <v>84</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E56" s="33"/>
       <c r="F56" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2566,17 +2566,17 @@
         <v>84</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E57" s="33"/>
       <c r="F57" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2584,17 +2584,17 @@
         <v>84</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E58" s="33"/>
       <c r="F58" s="32" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2602,17 +2602,17 @@
         <v>84</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E59" s="33"/>
       <c r="F59" s="32" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2620,17 +2620,17 @@
         <v>84</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E60" s="33"/>
       <c r="F60" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2638,17 +2638,17 @@
         <v>84</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E61" s="33"/>
       <c r="F61" s="32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2656,17 +2656,17 @@
         <v>84</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D62" s="29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E62" s="33"/>
       <c r="F62" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2674,13 +2674,13 @@
         <v>84</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D63" s="29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E63" s="33"/>
       <c r="F63" s="32" t="s">
@@ -2692,17 +2692,17 @@
         <v>84</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E64" s="33"/>
       <c r="F64" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2710,17 +2710,17 @@
         <v>84</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E65" s="34"/>
       <c r="F65" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2728,17 +2728,17 @@
         <v>84</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E66" s="34"/>
       <c r="F66" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2746,17 +2746,17 @@
         <v>84</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D67" s="29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E67" s="34"/>
       <c r="F67" s="35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2764,17 +2764,17 @@
         <v>84</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D68" s="29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E68" s="34"/>
       <c r="F68" s="35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2782,13 +2782,13 @@
         <v>84</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E69" s="34"/>
       <c r="F69" s="35" t="s">
@@ -2800,17 +2800,17 @@
         <v>84</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E70" s="34"/>
       <c r="F70" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2818,13 +2818,13 @@
         <v>84</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E71" s="34"/>
       <c r="F71" s="35" t="s">
@@ -2836,17 +2836,17 @@
         <v>84</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="E72" s="34"/>
       <c r="F72" s="35" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2854,17 +2854,17 @@
         <v>84</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E73" s="34"/>
       <c r="F73" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2872,17 +2872,17 @@
         <v>84</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D74" s="29" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E74" s="34"/>
       <c r="F74" s="35" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2890,13 +2890,13 @@
         <v>84</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E75" s="34"/>
       <c r="F75" s="35" t="s">
@@ -2908,17 +2908,17 @@
         <v>84</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D76" s="29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E76" s="34"/>
       <c r="F76" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2926,17 +2926,17 @@
         <v>84</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D77" s="29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E77" s="34"/>
       <c r="F77" s="35" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2944,17 +2944,17 @@
         <v>84</v>
       </c>
       <c r="B78" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E78" s="34"/>
       <c r="F78" s="35" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2962,17 +2962,17 @@
         <v>84</v>
       </c>
       <c r="B79" s="32" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E79" s="34"/>
       <c r="F79" s="35" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2980,17 +2980,17 @@
         <v>84</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E80" s="34"/>
       <c r="F80" s="35" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2998,17 +2998,17 @@
         <v>84</v>
       </c>
       <c r="B81" s="32" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E81" s="34"/>
       <c r="F81" s="35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3016,17 +3016,17 @@
         <v>84</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E82" s="34"/>
       <c r="F82" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3034,17 +3034,17 @@
         <v>84</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E83" s="34"/>
       <c r="F83" s="35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3052,17 +3052,17 @@
         <v>84</v>
       </c>
       <c r="B84" s="32" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E84" s="34"/>
       <c r="F84" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3070,17 +3070,17 @@
         <v>84</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E85" s="34"/>
       <c r="F85" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3088,17 +3088,17 @@
         <v>84</v>
       </c>
       <c r="B86" s="32" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E86" s="34"/>
       <c r="F86" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3106,17 +3106,17 @@
         <v>84</v>
       </c>
       <c r="B87" s="32" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D87" s="29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E87" s="34"/>
       <c r="F87" s="35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3141,7 +3141,7 @@
       </c>
       <c r="E89" s="34"/>
       <c r="G89" s="35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3159,7 +3159,7 @@
       </c>
       <c r="E90" s="34"/>
       <c r="G90" s="35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="E91" s="34"/>
       <c r="G91" s="35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="E92" s="34"/>
       <c r="G92" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="E93" s="34"/>
       <c r="G93" s="35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3231,7 +3231,7 @@
       </c>
       <c r="E94" s="34"/>
       <c r="G94" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="E95" s="34"/>
       <c r="G95" s="35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3267,7 +3267,7 @@
       </c>
       <c r="E96" s="34"/>
       <c r="G96" s="35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="E97" s="34"/>
       <c r="G97" s="35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3303,7 +3303,7 @@
       </c>
       <c r="E98" s="34"/>
       <c r="G98" s="35" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="E99" s="34"/>
       <c r="G99" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3339,7 +3339,7 @@
       </c>
       <c r="E100" s="34"/>
       <c r="G100" s="35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="E101" s="34"/>
       <c r="G101" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="102" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="E102" s="34"/>
       <c r="G102" s="35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="E103" s="34"/>
       <c r="G103" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="E104" s="34"/>
       <c r="G104" s="35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3429,7 +3429,7 @@
       </c>
       <c r="E105" s="34"/>
       <c r="G105" s="35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="E106" s="34"/>
       <c r="G106" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="E107" s="34"/>
       <c r="G107" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3483,7 +3483,7 @@
       </c>
       <c r="E108" s="34"/>
       <c r="G108" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="E109" s="34"/>
       <c r="G109" s="35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="E110" s="34"/>
       <c r="G110" s="35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="E111" s="34"/>
       <c r="G111" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="E112" s="34"/>
       <c r="G112" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="113" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="E113" s="34"/>
       <c r="G113" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3591,7 +3591,7 @@
       </c>
       <c r="E114" s="34"/>
       <c r="G114" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="E115" s="34"/>
       <c r="G115" s="35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3627,7 +3627,7 @@
       </c>
       <c r="E116" s="34"/>
       <c r="G116" s="35" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="E117" s="34"/>
       <c r="G117" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="E118" s="34"/>
       <c r="G118" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="E119" s="34"/>
       <c r="G119" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3699,7 +3699,7 @@
       </c>
       <c r="E120" s="24"/>
       <c r="G120" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3717,7 +3717,7 @@
       </c>
       <c r="E121" s="24"/>
       <c r="G121" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3735,7 +3735,7 @@
       </c>
       <c r="E122" s="24"/>
       <c r="G122" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="E123" s="24"/>
       <c r="G123" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="E124" s="24"/>
       <c r="G124" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="E125" s="24"/>
       <c r="G125" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3807,7 +3807,7 @@
       </c>
       <c r="E126" s="24"/>
       <c r="G126" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="E127" s="24"/>
       <c r="G127" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="E128" s="24"/>
       <c r="G128" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3863,7 +3863,7 @@
         <v>58</v>
       </c>
       <c r="G129" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3883,7 +3883,7 @@
         <v>59</v>
       </c>
       <c r="G130" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3903,7 +3903,7 @@
         <v>61</v>
       </c>
       <c r="G131" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3923,7 +3923,7 @@
         <v>60</v>
       </c>
       <c r="G132" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="E133" s="25"/>
       <c r="G133" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="E134" s="25"/>
       <c r="G134" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3976,12 +3976,12 @@
         <v>118</v>
       </c>
       <c r="G135" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A37:G64">
-    <sortCondition ref="B37:B64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:F87">
+    <sortCondition ref="B41:B87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3992,7 +3992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4019,10 +4019,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="C2">
         <v>20210722</v>

</xml_diff>